<commit_message>
Lots more work verifying bands
</commit_message>
<xml_diff>
--- a/data/intermediate_steps/bandstofix.xlsx
+++ b/data/intermediate_steps/bandstofix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raddick/Documents/GitHub/musical-folksonomy/data/intermediate_steps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9DD58A-A478-B84A-89B3-A2D02FE7B211}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F6E35A-DE15-4242-A2A9-D547A6B176F7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{DC525917-F686-F845-975F-4E45B1C7E8E0}"/>
   </bookViews>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7082D237-50E6-8C40-AD84-AF4B0C9D0833}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>